<commit_message>
added model description section in the README.md and updated compound_featurizer.py
</commit_message>
<xml_diff>
--- a/data/processed/IMT_Classification_Dataset_Processed_v3.xlsx
+++ b/data/processed/IMT_Classification_Dataset_Processed_v3.xlsx
@@ -1196,7 +1196,7 @@
         <v>10.33072101645395</v>
       </c>
       <c r="CP2" t="n">
-        <v>8.528538349421067</v>
+        <v>8.527722349421067</v>
       </c>
       <c r="CQ2" t="n">
         <v>12.08996707356846</v>
@@ -1487,7 +1487,7 @@
         <v>9.953087154069038</v>
       </c>
       <c r="CP3" t="n">
-        <v>13.6878685618895</v>
+        <v>13.6870525618895</v>
       </c>
       <c r="CQ3" t="n">
         <v>10.7470953027585</v>
@@ -1778,7 +1778,7 @@
         <v>18.52483317951593</v>
       </c>
       <c r="CP4" t="n">
-        <v>-7.676035875275144</v>
+        <v>-7.676851875275144</v>
       </c>
       <c r="CQ4" t="n">
         <v>13.43608826785714</v>
@@ -2069,7 +2069,7 @@
         <v>16.53026074663595</v>
       </c>
       <c r="CP5" t="n">
-        <v>6.587419111667807</v>
+        <v>6.586603111667807</v>
       </c>
       <c r="CQ5" t="n">
         <v>11.1468426036784</v>
@@ -2360,7 +2360,7 @@
         <v>16.12633861799301</v>
       </c>
       <c r="CP6" t="n">
-        <v>8.220232899913825</v>
+        <v>8.219416899913824</v>
       </c>
       <c r="CQ6" t="n">
         <v>9.504906710885679</v>
@@ -2651,7 +2651,7 @@
         <v>14.82361982478065</v>
       </c>
       <c r="CP7" t="n">
-        <v>8.689815517912123</v>
+        <v>8.688999517912123</v>
       </c>
       <c r="CQ7" t="n">
         <v>11.3325852903858</v>
@@ -2942,7 +2942,7 @@
         <v>9.072554617789944</v>
       </c>
       <c r="CP8" t="n">
-        <v>19.74753401445167</v>
+        <v>19.74671801445167</v>
       </c>
       <c r="CQ8" t="n">
         <v>9.289473631688375</v>
@@ -3233,7 +3233,7 @@
         <v>8.356268912906112</v>
       </c>
       <c r="CP9" t="n">
-        <v>13.60320030793818</v>
+        <v>13.60238430793818</v>
       </c>
       <c r="CQ9" t="n">
         <v>10.95913936342378</v>
@@ -3524,7 +3524,7 @@
         <v>11.92304527672917</v>
       </c>
       <c r="CP10" t="n">
-        <v>9.682226174561439</v>
+        <v>9.681410174561439</v>
       </c>
       <c r="CQ10" t="n">
         <v>13.63570221055</v>
@@ -3815,7 +3815,7 @@
         <v>12.95012665816691</v>
       </c>
       <c r="CP11" t="n">
-        <v>14.84329393525028</v>
+        <v>14.84247793525028</v>
       </c>
       <c r="CQ11" t="n">
         <v>10.684451982531</v>
@@ -4106,7 +4106,7 @@
         <v>5.884797567835469</v>
       </c>
       <c r="CP12" t="n">
-        <v>12.27682404284653</v>
+        <v>12.27600804284653</v>
       </c>
       <c r="CQ12" t="n">
         <v>12.45103828077785</v>
@@ -4397,7 +4397,7 @@
         <v>10.39061901846406</v>
       </c>
       <c r="CP13" t="n">
-        <v>12.71608635222468</v>
+        <v>12.71527035222468</v>
       </c>
       <c r="CQ13" t="n">
         <v>11.8369589623065</v>
@@ -4688,7 +4688,7 @@
         <v>26.96943700290353</v>
       </c>
       <c r="CP14" t="n">
-        <v>8.716856179848321</v>
+        <v>8.716040179848321</v>
       </c>
       <c r="CQ14" t="n">
         <v>9.163909322391588</v>
@@ -4979,7 +4979,7 @@
         <v>12.13441180473498</v>
       </c>
       <c r="CP15" t="n">
-        <v>7.702470483290037</v>
+        <v>7.701654483290037</v>
       </c>
       <c r="CQ15" t="n">
         <v>12.376680927</v>
@@ -5270,7 +5270,7 @@
         <v>8.928277399200802</v>
       </c>
       <c r="CP16" t="n">
-        <v>12.20257307207157</v>
+        <v>12.20175707207157</v>
       </c>
       <c r="CQ16" t="n">
         <v>10.493442375</v>
@@ -5561,7 +5561,7 @@
         <v>16.45802927081107</v>
       </c>
       <c r="CP17" t="n">
-        <v>7.077708085048883</v>
+        <v>7.076892085048883</v>
       </c>
       <c r="CQ17" t="n">
         <v>10.5390999057708</v>
@@ -5852,7 +5852,7 @@
         <v>10.45540180575522</v>
       </c>
       <c r="CP18" t="n">
-        <v>13.09203942466737</v>
+        <v>13.09122342466737</v>
       </c>
       <c r="CQ18" t="n">
         <v>12.4678747222902</v>
@@ -6143,7 +6143,7 @@
         <v>7.584741821723497</v>
       </c>
       <c r="CP19" t="n">
-        <v>15.86759846881216</v>
+        <v>15.86678246881216</v>
       </c>
       <c r="CQ19" t="n">
         <v>10.88259677438887</v>
@@ -6434,7 +6434,7 @@
         <v>8.878353973588865</v>
       </c>
       <c r="CP20" t="n">
-        <v>14.82850592180982</v>
+        <v>14.82768992180982</v>
       </c>
       <c r="CQ20" t="n">
         <v>10.77370787309688</v>
@@ -6725,7 +6725,7 @@
         <v>10.04325483835744</v>
       </c>
       <c r="CP21" t="n">
-        <v>11.8769575231632</v>
+        <v>11.8761415231632</v>
       </c>
       <c r="CQ21" t="n">
         <v>12.39349731496027</v>
@@ -7016,7 +7016,7 @@
         <v>12.02955729415996</v>
       </c>
       <c r="CP22" t="n">
-        <v>13.20362135268414</v>
+        <v>13.20280535268414</v>
       </c>
       <c r="CQ22" t="n">
         <v>14.09182804070857</v>
@@ -7307,7 +7307,7 @@
         <v>11.5272765658553</v>
       </c>
       <c r="CP23" t="n">
-        <v>3.448462516268151</v>
+        <v>3.447646516268151</v>
       </c>
       <c r="CQ23" t="n">
         <v>12.82763241676191</v>
@@ -7598,7 +7598,7 @@
         <v>10.52340939721885</v>
       </c>
       <c r="CP24" t="n">
-        <v>11.9472424123988</v>
+        <v>11.9464264123988</v>
       </c>
       <c r="CQ24" t="n">
         <v>13.19539481648091</v>
@@ -7889,7 +7889,7 @@
         <v>16.91859195346374</v>
       </c>
       <c r="CP25" t="n">
-        <v>13.84683322061992</v>
+        <v>13.84601722061992</v>
       </c>
       <c r="CQ25" t="n">
         <v>10.359518145816</v>
@@ -8180,7 +8180,7 @@
         <v>15.97487891136364</v>
       </c>
       <c r="CP26" t="n">
-        <v>0.5317661617894238</v>
+        <v>0.5309501617894234</v>
       </c>
       <c r="CQ26" t="n">
         <v>11.24771901709228</v>
@@ -8471,7 +8471,7 @@
         <v>17.60428926652129</v>
       </c>
       <c r="CP27" t="n">
-        <v>-6.443423393585506</v>
+        <v>-6.444239393585506</v>
       </c>
       <c r="CQ27" t="n">
         <v>12.96397470971429</v>
@@ -8762,7 +8762,7 @@
         <v>9.927379565898642</v>
       </c>
       <c r="CP28" t="n">
-        <v>10.33553114566295</v>
+        <v>10.33471514566295</v>
       </c>
       <c r="CQ28" t="n">
         <v>10.447063780671</v>
@@ -9053,7 +9053,7 @@
         <v>24.494682230869</v>
       </c>
       <c r="CP29" t="n">
-        <v>3.897989500064502</v>
+        <v>3.897173500064501</v>
       </c>
       <c r="CQ29" t="n">
         <v>11.457850275</v>
@@ -9344,7 +9344,7 @@
         <v>12.89182972726099</v>
       </c>
       <c r="CP30" t="n">
-        <v>7.009138226281549</v>
+        <v>7.008322226281549</v>
       </c>
       <c r="CQ30" t="n">
         <v>12.4375136714829</v>
@@ -9635,7 +9635,7 @@
         <v>11.87050287969283</v>
       </c>
       <c r="CP31" t="n">
-        <v>9.287718256504558</v>
+        <v>9.286902256504558</v>
       </c>
       <c r="CQ31" t="n">
         <v>13.187812950016</v>
@@ -9926,7 +9926,7 @@
         <v>52.80352596612941</v>
       </c>
       <c r="CP32" t="n">
-        <v>-6.054849433125765</v>
+        <v>-6.055665433125765</v>
       </c>
       <c r="CQ32" t="n">
         <v>13.16495658850511</v>
@@ -10217,7 +10217,7 @@
         <v>12.61227896838284</v>
       </c>
       <c r="CP33" t="n">
-        <v>17.24082192169813</v>
+        <v>17.24000592169813</v>
       </c>
       <c r="CQ33" t="n">
         <v>9.790637306394629</v>
@@ -10508,7 +10508,7 @@
         <v>16.81871161335582</v>
       </c>
       <c r="CP34" t="n">
-        <v>-1.555575230885184</v>
+        <v>-1.556391230885184</v>
       </c>
       <c r="CQ34" t="n">
         <v>11.59474464722905</v>
@@ -10799,7 +10799,7 @@
         <v>6.604164426157009</v>
       </c>
       <c r="CP35" t="n">
-        <v>12.94696497704856</v>
+        <v>12.94614897704856</v>
       </c>
       <c r="CQ35" t="n">
         <v>10.0723939220052</v>
@@ -11090,7 +11090,7 @@
         <v>18.28856630310757</v>
       </c>
       <c r="CP36" t="n">
-        <v>-1.862071256628939</v>
+        <v>-1.862887256628939</v>
       </c>
       <c r="CQ36" t="n">
         <v>11.08614965032081</v>
@@ -11381,7 +11381,7 @@
         <v>16.70494082987966</v>
       </c>
       <c r="CP37" t="n">
-        <v>3.645683612597614</v>
+        <v>3.644867612597613</v>
       </c>
       <c r="CQ37" t="n">
         <v>5.354962506455333</v>
@@ -11672,7 +11672,7 @@
         <v>42.15839073873798</v>
       </c>
       <c r="CP38" t="n">
-        <v>2.793838250997546</v>
+        <v>2.793022250997546</v>
       </c>
       <c r="CQ38" t="n">
         <v>14.31371621495424</v>
@@ -11963,7 +11963,7 @@
         <v>12.98191508403472</v>
       </c>
       <c r="CP39" t="n">
-        <v>8.693557461596765</v>
+        <v>8.692741461596764</v>
       </c>
       <c r="CQ39" t="n">
         <v>19.83169640448</v>
@@ -12254,7 +12254,7 @@
         <v>19.93375077701554</v>
       </c>
       <c r="CP40" t="n">
-        <v>14.07579222061901</v>
+        <v>14.07497622061901</v>
       </c>
       <c r="CQ40" t="n">
         <v>10.09073305588063</v>
@@ -12545,7 +12545,7 @@
         <v>86.95286016207095</v>
       </c>
       <c r="CP41" t="n">
-        <v>19.2294392221439</v>
+        <v>19.2286232221439</v>
       </c>
       <c r="CQ41" t="n">
         <v>8.523150058398592</v>
@@ -12836,7 +12836,7 @@
         <v>14.6143216297791</v>
       </c>
       <c r="CP42" t="n">
-        <v>14.87240280620565</v>
+        <v>14.87158680620565</v>
       </c>
       <c r="CQ42" t="n">
         <v>15.19925365664259</v>
@@ -13127,7 +13127,7 @@
         <v>14.49313992936021</v>
       </c>
       <c r="CP43" t="n">
-        <v>4.543935322423268</v>
+        <v>4.543119322423268</v>
       </c>
       <c r="CQ43" t="n">
         <v>11.7265219545334</v>
@@ -13418,7 +13418,7 @@
         <v>13.71742821003703</v>
       </c>
       <c r="CP44" t="n">
-        <v>6.302040114505752</v>
+        <v>6.301224114505752</v>
       </c>
       <c r="CQ44" t="n">
         <v>12.07680458789484</v>
@@ -13709,7 +13709,7 @@
         <v>15.87085139545565</v>
       </c>
       <c r="CP45" t="n">
-        <v>16.29670897049844</v>
+        <v>16.29589297049844</v>
       </c>
       <c r="CQ45" t="n">
         <v>14.6196608832</v>
@@ -14000,7 +14000,7 @@
         <v>14.86802807080926</v>
       </c>
       <c r="CP46" t="n">
-        <v>15.78998720196562</v>
+        <v>15.78917120196562</v>
       </c>
       <c r="CQ46" t="n">
         <v>14.2563879424</v>
@@ -14291,7 +14291,7 @@
         <v>15.43968433598971</v>
       </c>
       <c r="CP47" t="n">
-        <v>4.323371994492383</v>
+        <v>4.322555994492383</v>
       </c>
       <c r="CQ47" t="n">
         <v>11.63771114664327</v>
@@ -14582,7 +14582,7 @@
         <v>25.29036600615703</v>
       </c>
       <c r="CP48" t="n">
-        <v>-9.421215273906252</v>
+        <v>-9.422031273906253</v>
       </c>
       <c r="CQ48" t="n">
         <v>15.8411095308027</v>
@@ -14873,7 +14873,7 @@
         <v>32.40850484321987</v>
       </c>
       <c r="CP49" t="n">
-        <v>11.99306359533257</v>
+        <v>11.99224759533257</v>
       </c>
       <c r="CQ49" t="n">
         <v>11.92210068433334</v>
@@ -15164,7 +15164,7 @@
         <v>7.302539916353833</v>
       </c>
       <c r="CP50" t="n">
-        <v>5.167996439200875</v>
+        <v>5.167180439200875</v>
       </c>
       <c r="CQ50" t="n">
         <v>12.433788817164</v>
@@ -15455,7 +15455,7 @@
         <v>13.47223138270753</v>
       </c>
       <c r="CP51" t="n">
-        <v>15.29828212400971</v>
+        <v>15.29746612400971</v>
       </c>
       <c r="CQ51" t="n">
         <v>15.50908236629605</v>
@@ -15746,7 +15746,7 @@
         <v>13.76258293566901</v>
       </c>
       <c r="CP52" t="n">
-        <v>14.32181201804111</v>
+        <v>14.32099601804111</v>
       </c>
       <c r="CQ52" t="n">
         <v>17.9788129984</v>
@@ -16037,7 +16037,7 @@
         <v>13.44767254533834</v>
       </c>
       <c r="CP53" t="n">
-        <v>15.45234578654052</v>
+        <v>15.45152978654052</v>
       </c>
       <c r="CQ53" t="n">
         <v>10.985463567</v>
@@ -16328,7 +16328,7 @@
         <v>13.82941999768445</v>
       </c>
       <c r="CP54" t="n">
-        <v>10.81363919114045</v>
+        <v>10.81282319114045</v>
       </c>
       <c r="CQ54" t="n">
         <v>11.9474270956</v>
@@ -16619,7 +16619,7 @@
         <v>52.34150452588417</v>
       </c>
       <c r="CP55" t="n">
-        <v>10.09354149676122</v>
+        <v>10.09272549676122</v>
       </c>
       <c r="CQ55" t="n">
         <v>12.6555220448</v>
@@ -16910,7 +16910,7 @@
         <v>14.36657897971648</v>
       </c>
       <c r="CP56" t="n">
-        <v>12.57743162522831</v>
+        <v>12.57661562522831</v>
       </c>
       <c r="CQ56" t="n">
         <v>16.04708175811992</v>
@@ -17201,7 +17201,7 @@
         <v>24.88149532122058</v>
       </c>
       <c r="CP57" t="n">
-        <v>11.15788007002315</v>
+        <v>11.15706407002315</v>
       </c>
       <c r="CQ57" t="n">
         <v>13.21260373488533</v>
@@ -17492,7 +17492,7 @@
         <v>8.948894020851483</v>
       </c>
       <c r="CP58" t="n">
-        <v>11.32228882158181</v>
+        <v>11.32147282158181</v>
       </c>
       <c r="CQ58" t="n">
         <v>10.63636082506667</v>
@@ -17783,7 +17783,7 @@
         <v>20.6051521583596</v>
       </c>
       <c r="CP59" t="n">
-        <v>-0.9924920141513507</v>
+        <v>-0.9933080141513511</v>
       </c>
       <c r="CQ59" t="n">
         <v>13.57506224699978</v>
@@ -18074,7 +18074,7 @@
         <v>14.77226032577416</v>
       </c>
       <c r="CP60" t="n">
-        <v>9.293894007973538</v>
+        <v>9.293078007973538</v>
       </c>
       <c r="CQ60" t="n">
         <v>13.06376635733334</v>
@@ -18365,7 +18365,7 @@
         <v>11.83814873543771</v>
       </c>
       <c r="CP61" t="n">
-        <v>-4.529138565148171</v>
+        <v>4.926845434851829</v>
       </c>
       <c r="CQ61" t="n">
         <v>17.75676028609242</v>
@@ -18656,7 +18656,7 @@
         <v>9.744407414834548</v>
       </c>
       <c r="CP62" t="n">
-        <v>15.96948351987036</v>
+        <v>15.96866751987036</v>
       </c>
       <c r="CQ62" t="n">
         <v>10.119744747</v>
@@ -18947,7 +18947,7 @@
         <v>15.65505341042126</v>
       </c>
       <c r="CP63" t="n">
-        <v>-4.849438727360678</v>
+        <v>-4.850254727360679</v>
       </c>
       <c r="CQ63" t="n">
         <v>12.9499988227155</v>
@@ -19238,7 +19238,7 @@
         <v>11.82882777326081</v>
       </c>
       <c r="CP64" t="n">
-        <v>12.63329441698307</v>
+        <v>12.63247841698307</v>
       </c>
       <c r="CQ64" t="n">
         <v>10.1025276173166</v>
@@ -19529,7 +19529,7 @@
         <v>12.75925807445237</v>
       </c>
       <c r="CP65" t="n">
-        <v>14.58633482081348</v>
+        <v>14.58551882081348</v>
       </c>
       <c r="CQ65" t="n">
         <v>7.302019930769229</v>
@@ -19820,7 +19820,7 @@
         <v>17.06692830018083</v>
       </c>
       <c r="CP66" t="n">
-        <v>10.02960204266392</v>
+        <v>19.48558604266392</v>
       </c>
       <c r="CQ66" t="n">
         <v>24.774509559808</v>
@@ -20111,7 +20111,7 @@
         <v>19.93375077701554</v>
       </c>
       <c r="CP67" t="n">
-        <v>14.07579222061901</v>
+        <v>14.07497622061901</v>
       </c>
       <c r="CQ67" t="n">
         <v>10.09073305588063</v>
@@ -20402,7 +20402,7 @@
         <v>15.18189395193422</v>
       </c>
       <c r="CP68" t="n">
-        <v>-11.1100383821322</v>
+        <v>-11.1108543821322</v>
       </c>
       <c r="CQ68" t="n">
         <v>15.6472040715576</v>
@@ -20693,7 +20693,7 @@
         <v>15.9056206023324</v>
       </c>
       <c r="CP69" t="n">
-        <v>15.75418013459037</v>
+        <v>15.75336413459036</v>
       </c>
       <c r="CQ69" t="n">
         <v>14.92269944092234</v>
@@ -20984,7 +20984,7 @@
         <v>65.31100973779257</v>
       </c>
       <c r="CP70" t="n">
-        <v>-8.805123291487522</v>
+        <v>-8.805939291487523</v>
       </c>
       <c r="CQ70" t="n">
         <v>14.7090695899375</v>
@@ -21275,7 +21275,7 @@
         <v>53.9364774853067</v>
       </c>
       <c r="CP71" t="n">
-        <v>11.60737875966077</v>
+        <v>11.60656275966077</v>
       </c>
       <c r="CQ71" t="n">
         <v>13.59211638655543</v>
@@ -21566,7 +21566,7 @@
         <v>13.1519745082269</v>
       </c>
       <c r="CP72" t="n">
-        <v>15.29574710167907</v>
+        <v>15.29493110167907</v>
       </c>
       <c r="CQ72" t="n">
         <v>18.5680777625</v>
@@ -21857,7 +21857,7 @@
         <v>17.99936440392364</v>
       </c>
       <c r="CP73" t="n">
-        <v>11.5069940426437</v>
+        <v>20.9629780426437</v>
       </c>
       <c r="CQ73" t="n">
         <v>19.80769623796058</v>
@@ -22148,7 +22148,7 @@
         <v>52.622655221196</v>
       </c>
       <c r="CP74" t="n">
-        <v>9.415332820353818</v>
+        <v>9.414516820353818</v>
       </c>
       <c r="CQ74" t="n">
         <v>12.68433382885</v>
@@ -22439,7 +22439,7 @@
         <v>17.41470255776662</v>
       </c>
       <c r="CP75" t="n">
-        <v>4.799315875699561</v>
+        <v>4.79849987569956</v>
       </c>
       <c r="CQ75" t="n">
         <v>11.0099607405842</v>
@@ -22730,7 +22730,7 @@
         <v>14.28040263969531</v>
       </c>
       <c r="CP76" t="n">
-        <v>14.52551075782423</v>
+        <v>14.52469475782423</v>
       </c>
       <c r="CQ76" t="n">
         <v>14.95905455206335</v>
@@ -23021,7 +23021,7 @@
         <v>20.32129746245295</v>
       </c>
       <c r="CP77" t="n">
-        <v>14.6024202618712</v>
+        <v>14.6016042618712</v>
       </c>
       <c r="CQ77" t="n">
         <v>12.17007982222222</v>
@@ -23312,7 +23312,7 @@
         <v>32.72010801689695</v>
       </c>
       <c r="CP78" t="n">
-        <v>-12.4726220744997</v>
+        <v>-12.4734380744997</v>
       </c>
       <c r="CQ78" t="n">
         <v>13.12962951547705</v>
@@ -23603,7 +23603,7 @@
         <v>20.59470267846056</v>
       </c>
       <c r="CP79" t="n">
-        <v>4.862958240106172</v>
+        <v>4.862142240106172</v>
       </c>
       <c r="CQ79" t="n">
         <v>12.1450356695609</v>
@@ -23894,7 +23894,7 @@
         <v>18.01136117345864</v>
       </c>
       <c r="CP80" t="n">
-        <v>11.28363941934996</v>
+        <v>20.73962341934996</v>
       </c>
       <c r="CQ80" t="n">
         <v>20.057135813</v>
@@ -24185,7 +24185,7 @@
         <v>34.81229572598734</v>
       </c>
       <c r="CP81" t="n">
-        <v>16.24549168843643</v>
+        <v>16.24467568843643</v>
       </c>
       <c r="CQ81" t="n">
         <v>13.955744310976</v>
@@ -24476,7 +24476,7 @@
         <v>34.21912388746108</v>
       </c>
       <c r="CP82" t="n">
-        <v>-11.57917945615194</v>
+        <v>-11.57999545615194</v>
       </c>
       <c r="CQ82" t="n">
         <v>14.8797661626423</v>
@@ -24767,7 +24767,7 @@
         <v>11.63864003672866</v>
       </c>
       <c r="CP83" t="n">
-        <v>15.6736236704103</v>
+        <v>15.6728076704103</v>
       </c>
       <c r="CQ83" t="n">
         <v>9.684027430874998</v>
@@ -25058,7 +25058,7 @@
         <v>52.34433960307299</v>
       </c>
       <c r="CP84" t="n">
-        <v>11.09572360377686</v>
+        <v>11.09490760377686</v>
       </c>
       <c r="CQ84" t="n">
         <v>11.909488525</v>
@@ -25349,7 +25349,7 @@
         <v>26.96155853957426</v>
       </c>
       <c r="CP85" t="n">
-        <v>16.51398541368032</v>
+        <v>16.51316941368032</v>
       </c>
       <c r="CQ85" t="n">
         <v>16.44806029956319</v>
@@ -25640,7 +25640,7 @@
         <v>58.63344361191324</v>
       </c>
       <c r="CP86" t="n">
-        <v>3.247618306027917</v>
+        <v>3.246802306027917</v>
       </c>
       <c r="CQ86" t="n">
         <v>15.867007296</v>
@@ -25931,7 +25931,7 @@
         <v>60.27926086544328</v>
       </c>
       <c r="CP87" t="n">
-        <v>18.16418712353785</v>
+        <v>18.16337112353785</v>
       </c>
       <c r="CQ87" t="n">
         <v>9.373910789124997</v>
@@ -26222,7 +26222,7 @@
         <v>12.14401639841413</v>
       </c>
       <c r="CP88" t="n">
-        <v>15.41249395475325</v>
+        <v>15.41167795475325</v>
       </c>
       <c r="CQ88" t="n">
         <v>9.116230968999998</v>
@@ -26513,7 +26513,7 @@
         <v>13.73011237235636</v>
       </c>
       <c r="CP89" t="n">
-        <v>6.226360190833792</v>
+        <v>6.225544190833792</v>
       </c>
       <c r="CQ89" t="n">
         <v>12.10749252841774</v>
@@ -26804,7 +26804,7 @@
         <v>17.06517266439452</v>
       </c>
       <c r="CP90" t="n">
-        <v>10.06602369799984</v>
+        <v>19.52200769799984</v>
       </c>
       <c r="CQ90" t="n">
         <v>24.87982865936301</v>
@@ -27095,7 +27095,7 @@
         <v>12.70560182447126</v>
       </c>
       <c r="CP91" t="n">
-        <v>15.77328813913408</v>
+        <v>15.77247213913408</v>
       </c>
       <c r="CQ91" t="n">
         <v>13.50214992</v>
@@ -27386,7 +27386,7 @@
         <v>11.79603934229487</v>
       </c>
       <c r="CP92" t="n">
-        <v>10.25285130105554</v>
+        <v>10.25203530105554</v>
       </c>
       <c r="CQ92" t="n">
         <v>17.462413843992</v>
@@ -27677,7 +27677,7 @@
         <v>14.66938027485328</v>
       </c>
       <c r="CP93" t="n">
-        <v>14.41012531692454</v>
+        <v>14.40930931692454</v>
       </c>
       <c r="CQ93" t="n">
         <v>14.1918079849281</v>
@@ -27968,7 +27968,7 @@
         <v>52.43173749537478</v>
       </c>
       <c r="CP94" t="n">
-        <v>9.566470137439747</v>
+        <v>9.565654137439747</v>
       </c>
       <c r="CQ94" t="n">
         <v>12.856314272144</v>
@@ -28259,7 +28259,7 @@
         <v>20.36602752313157</v>
       </c>
       <c r="CP95" t="n">
-        <v>13.39582883582882</v>
+        <v>13.39501283582882</v>
       </c>
       <c r="CQ95" t="n">
         <v>12.459379671105</v>
@@ -28550,7 +28550,7 @@
         <v>6.255539463154387</v>
       </c>
       <c r="CP96" t="n">
-        <v>12.94526351324791</v>
+        <v>12.94444751324791</v>
       </c>
       <c r="CQ96" t="n">
         <v>10.5118667260146</v>
@@ -28841,7 +28841,7 @@
         <v>13.77380601271575</v>
       </c>
       <c r="CP97" t="n">
-        <v>14.38062875554606</v>
+        <v>14.37981275554606</v>
       </c>
       <c r="CQ97" t="n">
         <v>9.641401444553715</v>
@@ -29132,7 +29132,7 @@
         <v>51.99623536116106</v>
       </c>
       <c r="CP98" t="n">
-        <v>12.31178688869684</v>
+        <v>12.31097088869684</v>
       </c>
       <c r="CQ98" t="n">
         <v>10.3956804042</v>
@@ -29423,7 +29423,7 @@
         <v>14.28040263969531</v>
       </c>
       <c r="CP99" t="n">
-        <v>14.52551075782423</v>
+        <v>14.52469475782423</v>
       </c>
       <c r="CQ99" t="n">
         <v>14.95905455206335</v>
@@ -29714,7 +29714,7 @@
         <v>13.86704549360247</v>
       </c>
       <c r="CP100" t="n">
-        <v>2.21743250255447</v>
+        <v>2.216616502554469</v>
       </c>
       <c r="CQ100" t="n">
         <v>12.23981774340195</v>
@@ -30005,7 +30005,7 @@
         <v>16.99669511730325</v>
       </c>
       <c r="CP101" t="n">
-        <v>6.835396731998358</v>
+        <v>6.834580731998358</v>
       </c>
       <c r="CQ101" t="n">
         <v>9.263051370495001</v>
@@ -30296,7 +30296,7 @@
         <v>17.27675067694737</v>
       </c>
       <c r="CP102" t="n">
-        <v>14.8313806652595</v>
+        <v>14.8305646652595</v>
       </c>
       <c r="CQ102" t="n">
         <v>11.94335914020373</v>
@@ -30587,7 +30587,7 @@
         <v>27.31683529867346</v>
       </c>
       <c r="CP103" t="n">
-        <v>17.03970037639023</v>
+        <v>17.03888437639023</v>
       </c>
       <c r="CQ103" t="n">
         <v>14.797038793892</v>
@@ -30878,7 +30878,7 @@
         <v>8.698260289434952</v>
       </c>
       <c r="CP104" t="n">
-        <v>15.48403314782841</v>
+        <v>15.48321714782841</v>
       </c>
       <c r="CQ104" t="n">
         <v>14.500009266625</v>
@@ -31169,7 +31169,7 @@
         <v>16.08861623599942</v>
       </c>
       <c r="CP105" t="n">
-        <v>-3.382876930538476</v>
+        <v>-3.383692930538476</v>
       </c>
       <c r="CQ105" t="n">
         <v>13.21481513635714</v>
@@ -31460,7 +31460,7 @@
         <v>9.273797311125403</v>
       </c>
       <c r="CP106" t="n">
-        <v>11.83941220530502</v>
+        <v>11.83859620530502</v>
       </c>
       <c r="CQ106" t="n">
         <v>12.107331</v>
@@ -31751,7 +31751,7 @@
         <v>13.23714341140638</v>
       </c>
       <c r="CP107" t="n">
-        <v>11.07526065832683</v>
+        <v>11.07444465832683</v>
       </c>
       <c r="CQ107" t="n">
         <v>10.4307522778017</v>
@@ -32042,7 +32042,7 @@
         <v>13.2852322817887</v>
       </c>
       <c r="CP108" t="n">
-        <v>-5.286432633119927</v>
+        <v>-5.287248633119927</v>
       </c>
       <c r="CQ108" t="n">
         <v>9.367529904017855</v>
@@ -32333,7 +32333,7 @@
         <v>18.21694487869566</v>
       </c>
       <c r="CP109" t="n">
-        <v>6.199214287184801</v>
+        <v>6.1983982871848</v>
       </c>
       <c r="CQ109" t="n">
         <v>13.3641852049915</v>
@@ -32624,7 +32624,7 @@
         <v>13.83870344381146</v>
       </c>
       <c r="CP110" t="n">
-        <v>10.82657886667493</v>
+        <v>10.82576286667492</v>
       </c>
       <c r="CQ110" t="n">
         <v>12.014148984288</v>
@@ -32915,7 +32915,7 @@
         <v>13.83121607343389</v>
       </c>
       <c r="CP111" t="n">
-        <v>10.75899021596991</v>
+        <v>10.75817421596991</v>
       </c>
       <c r="CQ111" t="n">
         <v>11.96269068794811</v>
@@ -33206,7 +33206,7 @@
         <v>19.0862795792284</v>
       </c>
       <c r="CP112" t="n">
-        <v>4.966062812817715</v>
+        <v>4.965246812817715</v>
       </c>
       <c r="CQ112" t="n">
         <v>12.92740987656857</v>
@@ -33497,7 +33497,7 @@
         <v>14.37591627567882</v>
       </c>
       <c r="CP113" t="n">
-        <v>13.53814212393809</v>
+        <v>13.53732612393809</v>
       </c>
       <c r="CQ113" t="n">
         <v>16.2771336</v>
@@ -33788,7 +33788,7 @@
         <v>12.06047675027972</v>
       </c>
       <c r="CP114" t="n">
-        <v>16.10319101149364</v>
+        <v>16.10237501149364</v>
       </c>
       <c r="CQ114" t="n">
         <v>11.7610069416</v>
@@ -34079,7 +34079,7 @@
         <v>20.3770656121452</v>
       </c>
       <c r="CP115" t="n">
-        <v>18.83191463025619</v>
+        <v>18.83109863025619</v>
       </c>
       <c r="CQ115" t="n">
         <v>13.9152888568</v>
@@ -34370,7 +34370,7 @@
         <v>15.31120520480402</v>
       </c>
       <c r="CP116" t="n">
-        <v>-1.295007763627719</v>
+        <v>-1.29582376362772</v>
       </c>
       <c r="CQ116" t="n">
         <v>13.63528800043429</v>
@@ -34661,7 +34661,7 @@
         <v>32.79222260007773</v>
       </c>
       <c r="CP117" t="n">
-        <v>-14.02097574104298</v>
+        <v>-14.02179174104298</v>
       </c>
       <c r="CQ117" t="n">
         <v>13.9543400587264</v>
@@ -34952,7 +34952,7 @@
         <v>10.70017782586434</v>
       </c>
       <c r="CP118" t="n">
-        <v>2.871666985693134</v>
+        <v>12.32765098569313</v>
       </c>
       <c r="CQ118" t="n">
         <v>13.32791682250341</v>
@@ -35243,7 +35243,7 @@
         <v>16.46766227896141</v>
       </c>
       <c r="CP119" t="n">
-        <v>8.881110477012001</v>
+        <v>8.880294477012001</v>
       </c>
       <c r="CQ119" t="n">
         <v>13.19882100050514</v>
@@ -35534,7 +35534,7 @@
         <v>14.91299089744727</v>
       </c>
       <c r="CP120" t="n">
-        <v>-7.58139826319346</v>
+        <v>-7.58221426319346</v>
       </c>
       <c r="CQ120" t="n">
         <v>11.55365956333586</v>
@@ -35825,7 +35825,7 @@
         <v>16.62970066391833</v>
       </c>
       <c r="CP121" t="n">
-        <v>8.641850786724303</v>
+        <v>8.641034786724303</v>
       </c>
       <c r="CQ121" t="n">
         <v>9.995143347194865</v>
@@ -36116,7 +36116,7 @@
         <v>14.56719394594053</v>
       </c>
       <c r="CP122" t="n">
-        <v>-4.933417092110805</v>
+        <v>-4.934233092110805</v>
       </c>
       <c r="CQ122" t="n">
         <v>11.72680120315714</v>
@@ -36407,7 +36407,7 @@
         <v>9.409743417201106</v>
       </c>
       <c r="CP123" t="n">
-        <v>12.93436117462137</v>
+        <v>12.93354517462137</v>
       </c>
       <c r="CQ123" t="n">
         <v>14.98613726358587</v>
@@ -36698,7 +36698,7 @@
         <v>9.56283217352512</v>
       </c>
       <c r="CP124" t="n">
-        <v>13.69563665702669</v>
+        <v>23.15162065702669</v>
       </c>
       <c r="CQ124" t="n">
         <v>15.08115817819984</v>
@@ -36989,7 +36989,7 @@
         <v>10.98786853507603</v>
       </c>
       <c r="CP125" t="n">
-        <v>15.32768913986451</v>
+        <v>15.32687313986451</v>
       </c>
       <c r="CQ125" t="n">
         <v>10.98923718019462</v>
@@ -37280,7 +37280,7 @@
         <v>16.63212427422593</v>
       </c>
       <c r="CP126" t="n">
-        <v>8.528116748417542</v>
+        <v>8.527300748417542</v>
       </c>
       <c r="CQ126" t="n">
         <v>10.01375619645705</v>
@@ -37571,7 +37571,7 @@
         <v>39.98615701173624</v>
       </c>
       <c r="CP127" t="n">
-        <v>11.0211866950888</v>
+        <v>11.0203706950888</v>
       </c>
       <c r="CQ127" t="n">
         <v>13.90358883684604</v>
@@ -37862,7 +37862,7 @@
         <v>14.15447399937196</v>
       </c>
       <c r="CP128" t="n">
-        <v>2.275443302649308</v>
+        <v>2.274627302649308</v>
       </c>
       <c r="CQ128" t="n">
         <v>19.79020364751353</v>
@@ -38153,7 +38153,7 @@
         <v>13.50214226748114</v>
       </c>
       <c r="CP129" t="n">
-        <v>12.62991151600431</v>
+        <v>12.62909551600431</v>
       </c>
       <c r="CQ129" t="n">
         <v>10.04025606293397</v>
@@ -38444,7 +38444,7 @@
         <v>14.96533650189407</v>
       </c>
       <c r="CP130" t="n">
-        <v>10.30662023207008</v>
+        <v>10.30580423207008</v>
       </c>
       <c r="CQ130" t="n">
         <v>8.510004814365116</v>
@@ -38735,7 +38735,7 @@
         <v>16.58960558852893</v>
       </c>
       <c r="CP131" t="n">
-        <v>7.383202797336414</v>
+        <v>7.382386797336413</v>
       </c>
       <c r="CQ131" t="n">
         <v>9.693805070284174</v>
@@ -39026,7 +39026,7 @@
         <v>16.58618512936862</v>
       </c>
       <c r="CP132" t="n">
-        <v>7.431751954192498</v>
+        <v>7.430935954192497</v>
       </c>
       <c r="CQ132" t="n">
         <v>9.668662040325902</v>
@@ -39317,7 +39317,7 @@
         <v>10.30320840700934</v>
       </c>
       <c r="CP133" t="n">
-        <v>-4.92426414777195</v>
+        <v>-4.925080147771951</v>
       </c>
       <c r="CQ133" t="n">
         <v>12.98277636149744</v>
@@ -39608,7 +39608,7 @@
         <v>16.5881156251672</v>
       </c>
       <c r="CP134" t="n">
-        <v>7.422557164100011</v>
+        <v>7.421741164100011</v>
       </c>
       <c r="CQ134" t="n">
         <v>9.682841979403555</v>
@@ -39899,7 +39899,7 @@
         <v>11.05179778510488</v>
       </c>
       <c r="CP135" t="n">
-        <v>16.08239710823262</v>
+        <v>16.08158110823262</v>
       </c>
       <c r="CQ135" t="n">
         <v>10.46521609194463</v>
@@ -40190,7 +40190,7 @@
         <v>16.63433313176809</v>
       </c>
       <c r="CP136" t="n">
-        <v>8.545165244604192</v>
+        <v>8.544349244604192</v>
       </c>
       <c r="CQ136" t="n">
         <v>10.03076006129224</v>
@@ -40481,7 +40481,7 @@
         <v>11.68989187974098</v>
       </c>
       <c r="CP137" t="n">
-        <v>12.45592542638215</v>
+        <v>21.91190942638215</v>
       </c>
       <c r="CQ137" t="n">
         <v>13.89300065427965</v>
@@ -40772,7 +40772,7 @@
         <v>12.94491337177938</v>
       </c>
       <c r="CP138" t="n">
-        <v>15.52693280517861</v>
+        <v>15.52611680517861</v>
       </c>
       <c r="CQ138" t="n">
         <v>9.99693223979979</v>
@@ -41063,7 +41063,7 @@
         <v>16.59207915276189</v>
       </c>
       <c r="CP139" t="n">
-        <v>7.563509443874139</v>
+        <v>7.562693443874139</v>
       </c>
       <c r="CQ139" t="n">
         <v>9.712042030878864</v>
@@ -41354,7 +41354,7 @@
         <v>28.92844421191396</v>
       </c>
       <c r="CP140" t="n">
-        <v>10.04360003329252</v>
+        <v>10.04278403329252</v>
       </c>
       <c r="CQ140" t="n">
         <v>11.55567265214666</v>
@@ -41645,7 +41645,7 @@
         <v>16.99148115645173</v>
       </c>
       <c r="CP141" t="n">
-        <v>-14.42356818666003</v>
+        <v>-14.42438418666003</v>
       </c>
       <c r="CQ141" t="n">
         <v>10.01430756823715</v>
@@ -41936,7 +41936,7 @@
         <v>14.15447399937196</v>
       </c>
       <c r="CP142" t="n">
-        <v>2.275443302649308</v>
+        <v>2.274627302649308</v>
       </c>
       <c r="CQ142" t="n">
         <v>19.79020364751353</v>
@@ -42227,7 +42227,7 @@
         <v>15.94941068856103</v>
       </c>
       <c r="CP143" t="n">
-        <v>10.42584912335981</v>
+        <v>10.42503312335981</v>
       </c>
       <c r="CQ143" t="n">
         <v>11.0304292754252</v>
@@ -42518,7 +42518,7 @@
         <v>10.26428037843544</v>
       </c>
       <c r="CP144" t="n">
-        <v>8.81809541605719</v>
+        <v>8.81727941605719</v>
       </c>
       <c r="CQ144" t="n">
         <v>12.69274899342729</v>
@@ -42809,7 +42809,7 @@
         <v>16.58994676738826</v>
       </c>
       <c r="CP145" t="n">
-        <v>7.601272703591714</v>
+        <v>7.600456703591714</v>
       </c>
       <c r="CQ145" t="n">
         <v>9.696317779209235</v>
@@ -43100,7 +43100,7 @@
         <v>12.5824307629021</v>
       </c>
       <c r="CP146" t="n">
-        <v>2.239839617186466</v>
+        <v>2.239023617186466</v>
       </c>
       <c r="CQ146" t="n">
         <v>9.571252955879196</v>
@@ -43391,7 +43391,7 @@
         <v>13.50406780341771</v>
       </c>
       <c r="CP147" t="n">
-        <v>-5.919083467848749</v>
+        <v>3.536900532151252</v>
       </c>
       <c r="CQ147" t="n">
         <v>21.7305024679944</v>
@@ -43682,7 +43682,7 @@
         <v>15.98908219439416</v>
       </c>
       <c r="CP148" t="n">
-        <v>-915.1488750505277</v>
+        <v>-915.1496910505277</v>
       </c>
       <c r="CQ148" t="n">
         <v>9.451653015342368</v>
@@ -43973,7 +43973,7 @@
         <v>19.89068054440046</v>
       </c>
       <c r="CP149" t="n">
-        <v>-1.23111920357849</v>
+        <v>-1.23193520357849</v>
       </c>
       <c r="CQ149" t="n">
         <v>10.518436314</v>
@@ -44264,7 +44264,7 @@
         <v>16.61346966568117</v>
       </c>
       <c r="CP150" t="n">
-        <v>7.647574263777817</v>
+        <v>7.646758263777817</v>
       </c>
       <c r="CQ150" t="n">
         <v>9.871673688442343</v>
@@ -44555,7 +44555,7 @@
         <v>7.859266311413077</v>
       </c>
       <c r="CP151" t="n">
-        <v>4.997485173870698</v>
+        <v>14.4534691738707</v>
       </c>
       <c r="CQ151" t="n">
         <v>16.87230790922946</v>
@@ -44846,7 +44846,7 @@
         <v>14.44527231426382</v>
       </c>
       <c r="CP152" t="n">
-        <v>-11.15956891725489</v>
+        <v>-11.16038491725489</v>
       </c>
       <c r="CQ152" t="n">
         <v>11.8032016936286</v>
@@ -45137,7 +45137,7 @@
         <v>17.93370884263274</v>
       </c>
       <c r="CP153" t="n">
-        <v>3.315035011613712</v>
+        <v>3.983726976215482</v>
       </c>
       <c r="CQ153" t="n">
         <v>9.999284830965612</v>
@@ -45428,7 +45428,7 @@
         <v>15.95770770865147</v>
       </c>
       <c r="CP154" t="n">
-        <v>10.39576638563782</v>
+        <v>10.39495038563782</v>
       </c>
       <c r="CQ154" t="n">
         <v>11.1057827084574</v>
@@ -45719,7 +45719,7 @@
         <v>8.618194760382028</v>
       </c>
       <c r="CP155" t="n">
-        <v>14.88051824900841</v>
+        <v>14.87970224900841</v>
       </c>
       <c r="CQ155" t="n">
         <v>11.704715124375</v>
@@ -46010,7 +46010,7 @@
         <v>14.24457973704767</v>
       </c>
       <c r="CP156" t="n">
-        <v>-6.996635915794053</v>
+        <v>-6.997451915794053</v>
       </c>
       <c r="CQ156" t="n">
         <v>10.23755254132694</v>
@@ -46301,7 +46301,7 @@
         <v>13.82965388345842</v>
       </c>
       <c r="CP157" t="n">
-        <v>10.59043258506153</v>
+        <v>10.58961658506153</v>
       </c>
       <c r="CQ157" t="n">
         <v>11.04010682812637</v>
@@ -46592,7 +46592,7 @@
         <v>16.63796145869878</v>
       </c>
       <c r="CP158" t="n">
-        <v>8.604668572228222</v>
+        <v>8.603852572228222</v>
       </c>
       <c r="CQ158" t="n">
         <v>10.05877470732488</v>
@@ -46883,7 +46883,7 @@
         <v>16.5917816230589</v>
       </c>
       <c r="CP159" t="n">
-        <v>7.508684579640144</v>
+        <v>7.507868579640143</v>
       </c>
       <c r="CQ159" t="n">
         <v>9.709846000992027</v>
@@ -47174,7 +47174,7 @@
         <v>17.93370884263274</v>
       </c>
       <c r="CP160" t="n">
-        <v>3.315035011613712</v>
+        <v>3.983726976215482</v>
       </c>
       <c r="CQ160" t="n">
         <v>10.57499932414594</v>
@@ -47465,7 +47465,7 @@
         <v>14.00601003336779</v>
       </c>
       <c r="CP161" t="n">
-        <v>2.367208745729396</v>
+        <v>2.366392745729396</v>
       </c>
       <c r="CQ161" t="n">
         <v>11.19557510896258</v>
@@ -47756,7 +47756,7 @@
         <v>16.64443440337321</v>
       </c>
       <c r="CP162" t="n">
-        <v>8.611017037967938</v>
+        <v>8.610201037967938</v>
       </c>
       <c r="CQ162" t="n">
         <v>10.10901253187971</v>
@@ -48047,7 +48047,7 @@
         <v>24.76841834378966</v>
       </c>
       <c r="CP163" t="n">
-        <v>15.72754063753623</v>
+        <v>15.72672463753623</v>
       </c>
       <c r="CQ163" t="n">
         <v>10.72334910239958</v>
@@ -48338,7 +48338,7 @@
         <v>16.65461976927839</v>
       </c>
       <c r="CP164" t="n">
-        <v>1.438346604327499</v>
+        <v>1.437530604327499</v>
       </c>
       <c r="CQ164" t="n">
         <v>10.1887427901083</v>
@@ -48629,7 +48629,7 @@
         <v>16.7504568636591</v>
       </c>
       <c r="CP165" t="n">
-        <v>-5.015021793335554</v>
+        <v>-5.015837793335554</v>
       </c>
       <c r="CQ165" t="n">
         <v>10.55345680641366</v>
@@ -48920,7 +48920,7 @@
         <v>15.94037356959455</v>
       </c>
       <c r="CP166" t="n">
-        <v>10.39466287840977</v>
+        <v>10.39384687840977</v>
       </c>
       <c r="CQ166" t="n">
         <v>10.97175185476754</v>
@@ -49211,7 +49211,7 @@
         <v>51.80571254629766</v>
       </c>
       <c r="CP167" t="n">
-        <v>-2.663070035662293</v>
+        <v>6.792913964337708</v>
       </c>
       <c r="CQ167" t="n">
         <v>19.08739798670936</v>
@@ -49502,7 +49502,7 @@
         <v>13.44529990742059</v>
       </c>
       <c r="CP168" t="n">
-        <v>-6.882085143883581</v>
+        <v>2.57389885611642</v>
       </c>
       <c r="CQ168" t="n">
         <v>21.94021942489053</v>
@@ -49793,7 +49793,7 @@
         <v>16.59890997769964</v>
       </c>
       <c r="CP169" t="n">
-        <v>7.387353343037568</v>
+        <v>7.386537343037568</v>
       </c>
       <c r="CQ169" t="n">
         <v>9.762642148383927</v>
@@ -50084,7 +50084,7 @@
         <v>14.13382808778058</v>
       </c>
       <c r="CP170" t="n">
-        <v>8.670629882990603</v>
+        <v>8.669813882990603</v>
       </c>
       <c r="CQ170" t="n">
         <v>10.05530067731169</v>
@@ -50375,7 +50375,7 @@
         <v>10.96918661708149</v>
       </c>
       <c r="CP171" t="n">
-        <v>12.78944044257534</v>
+        <v>12.78862444257534</v>
       </c>
       <c r="CQ171" t="n">
         <v>10.86619143614286</v>
@@ -50666,7 +50666,7 @@
         <v>13.4643304404452</v>
       </c>
       <c r="CP172" t="n">
-        <v>13.91415495005348</v>
+        <v>13.91333895005348</v>
       </c>
       <c r="CQ172" t="n">
         <v>10.21662244808293</v>
@@ -50957,7 +50957,7 @@
         <v>11.06577628822614</v>
       </c>
       <c r="CP173" t="n">
-        <v>17.8024990163471</v>
+        <v>17.8016830163471</v>
       </c>
       <c r="CQ173" t="n">
         <v>9.817068105142857</v>
@@ -51248,7 +51248,7 @@
         <v>16.60110269684154</v>
       </c>
       <c r="CP174" t="n">
-        <v>7.51565466325806</v>
+        <v>7.514838663258059</v>
       </c>
       <c r="CQ174" t="n">
         <v>9.778959476652243</v>
@@ -51539,7 +51539,7 @@
         <v>16.00069976423015</v>
       </c>
       <c r="CP175" t="n">
-        <v>-17.29903399876845</v>
+        <v>-17.29984999876845</v>
       </c>
       <c r="CQ175" t="n">
         <v>11.40634264085489</v>
@@ -51830,7 +51830,7 @@
         <v>58.59293991783679</v>
       </c>
       <c r="CP176" t="n">
-        <v>-12.46620407568821</v>
+        <v>-12.46702007568821</v>
       </c>
       <c r="CQ176" t="n">
         <v>11.49483077827375</v>
@@ -52121,7 +52121,7 @@
         <v>16.61102284828911</v>
       </c>
       <c r="CP177" t="n">
-        <v>7.531931260990568</v>
+        <v>7.531115260990568</v>
       </c>
       <c r="CQ177" t="n">
         <v>9.853237374589336</v>
@@ -52412,7 +52412,7 @@
         <v>13.03622163607541</v>
       </c>
       <c r="CP178" t="n">
-        <v>15.30093690301311</v>
+        <v>15.30012090301311</v>
       </c>
       <c r="CQ178" t="n">
         <v>10.03134767999574</v>
@@ -52703,7 +52703,7 @@
         <v>16.63298268832751</v>
       </c>
       <c r="CP179" t="n">
-        <v>8.609994690970638</v>
+        <v>8.609178690970637</v>
       </c>
       <c r="CQ179" t="n">
         <v>10.02035972999621</v>
@@ -52994,7 +52994,7 @@
         <v>7.864049328061065</v>
       </c>
       <c r="CP180" t="n">
-        <v>4.71711388634967</v>
+        <v>14.17309788634967</v>
       </c>
       <c r="CQ180" t="n">
         <v>17.05205445072186</v>
@@ -53285,7 +53285,7 @@
         <v>13.00173164022466</v>
       </c>
       <c r="CP181" t="n">
-        <v>-5.623831139158788</v>
+        <v>-5.624647139158788</v>
       </c>
       <c r="CQ181" t="n">
         <v>12.01136311806392</v>
@@ -53576,7 +53576,7 @@
         <v>16.75548951451688</v>
       </c>
       <c r="CP182" t="n">
-        <v>-5.240157923707637</v>
+        <v>-5.240973923707638</v>
       </c>
       <c r="CQ182" t="n">
         <v>10.59872495379975</v>
@@ -53867,7 +53867,7 @@
         <v>13.07505583158088</v>
       </c>
       <c r="CP183" t="n">
-        <v>12.70735568661238</v>
+        <v>12.70653968661238</v>
       </c>
       <c r="CQ183" t="n">
         <v>12.69719141591854</v>
@@ -54158,7 +54158,7 @@
         <v>14.0403814975846</v>
       </c>
       <c r="CP184" t="n">
-        <v>1.90568070986949</v>
+        <v>1.904864709869489</v>
       </c>
       <c r="CQ184" t="n">
         <v>11.50905035963304</v>
@@ -54449,7 +54449,7 @@
         <v>15.93968142007486</v>
       </c>
       <c r="CP185" t="n">
-        <v>10.43635380722969</v>
+        <v>10.43553780722969</v>
       </c>
       <c r="CQ185" t="n">
         <v>10.96483065827978</v>
@@ -54740,7 +54740,7 @@
         <v>9.639638210146686</v>
       </c>
       <c r="CP186" t="n">
-        <v>14.60021098929582</v>
+        <v>14.59939498929582</v>
       </c>
       <c r="CQ186" t="n">
         <v>16.994415411</v>
@@ -55031,7 +55031,7 @@
         <v>16.59950823414829</v>
       </c>
       <c r="CP187" t="n">
-        <v>7.579803374987769</v>
+        <v>7.578987374987769</v>
       </c>
       <c r="CQ187" t="n">
         <v>9.767090527237547</v>
@@ -55322,7 +55322,7 @@
         <v>13.45959704887719</v>
       </c>
       <c r="CP188" t="n">
-        <v>14.39869779607763</v>
+        <v>14.39788179607763</v>
       </c>
       <c r="CQ188" t="n">
         <v>9.821617900445073</v>
@@ -55613,7 +55613,7 @@
         <v>9.677301246396823</v>
       </c>
       <c r="CP189" t="n">
-        <v>20.01180282518023</v>
+        <v>20.01098682518023</v>
       </c>
       <c r="CQ189" t="n">
         <v>8.446042127125002</v>
@@ -55904,7 +55904,7 @@
         <v>10.19762836903829</v>
       </c>
       <c r="CP190" t="n">
-        <v>9.366602937033809</v>
+        <v>9.365786937033809</v>
       </c>
       <c r="CQ190" t="n">
         <v>12.5628302225055</v>
@@ -56195,7 +56195,7 @@
         <v>16.19770621287739</v>
       </c>
       <c r="CP191" t="n">
-        <v>-18.20143022975832</v>
+        <v>-18.20224622975832</v>
       </c>
       <c r="CQ191" t="n">
         <v>10.9591256392764</v>
@@ -56486,7 +56486,7 @@
         <v>15.95467180623404</v>
       </c>
       <c r="CP192" t="n">
-        <v>10.46166013160131</v>
+        <v>10.46084413160131</v>
       </c>
       <c r="CQ192" t="n">
         <v>11.07937351667175</v>
@@ -56777,7 +56777,7 @@
         <v>24.77768507747149</v>
       </c>
       <c r="CP193" t="n">
-        <v>15.53764132264759</v>
+        <v>15.53682532264759</v>
       </c>
       <c r="CQ193" t="n">
         <v>10.67711976382482</v>
@@ -57068,7 +57068,7 @@
         <v>16.61481224485347</v>
       </c>
       <c r="CP194" t="n">
-        <v>7.564797718543676</v>
+        <v>7.563981718543675</v>
       </c>
       <c r="CQ194" t="n">
         <v>9.881809318471706</v>
@@ -57359,7 +57359,7 @@
         <v>18.06711847015571</v>
       </c>
       <c r="CP195" t="n">
-        <v>1.970785444817324</v>
+        <v>1.969969444817323</v>
       </c>
       <c r="CQ195" t="n">
         <v>11.88055409054227</v>
@@ -57650,7 +57650,7 @@
         <v>9.83012221073831</v>
       </c>
       <c r="CP196" t="n">
-        <v>13.46312430718785</v>
+        <v>22.91910830718785</v>
       </c>
       <c r="CQ196" t="n">
         <v>15.14965854375</v>
@@ -57941,7 +57941,7 @@
         <v>13.75707479413553</v>
       </c>
       <c r="CP197" t="n">
-        <v>12.20043434974242</v>
+        <v>12.19961834974242</v>
       </c>
       <c r="CQ197" t="n">
         <v>10.00261822444712</v>
@@ -58232,7 +58232,7 @@
         <v>14.01899911466746</v>
       </c>
       <c r="CP198" t="n">
-        <v>11.77777627679629</v>
+        <v>11.77696027679629</v>
       </c>
       <c r="CQ198" t="n">
         <v>11.3184088242264</v>
@@ -58523,7 +58523,7 @@
         <v>13.95514452413227</v>
       </c>
       <c r="CP199" t="n">
-        <v>12.58078209409998</v>
+        <v>12.57996609409998</v>
       </c>
       <c r="CQ199" t="n">
         <v>10.758068450129</v>
@@ -58814,7 +58814,7 @@
         <v>17.91290796027692</v>
       </c>
       <c r="CP200" t="n">
-        <v>-20.42641270958305</v>
+        <v>-20.42722870958305</v>
       </c>
       <c r="CQ200" t="n">
         <v>11.60347945649925</v>
@@ -59105,7 +59105,7 @@
         <v>17.62126873825136</v>
       </c>
       <c r="CP201" t="n">
-        <v>-22.1747705620908</v>
+        <v>-22.1755865620908</v>
       </c>
       <c r="CQ201" t="n">
         <v>11.60529215798984</v>
@@ -59396,7 +59396,7 @@
         <v>16.46804478710224</v>
       </c>
       <c r="CP202" t="n">
-        <v>6.349085696591781</v>
+        <v>6.348269696591781</v>
       </c>
       <c r="CQ202" t="n">
         <v>10.7600951587344</v>
@@ -59687,7 +59687,7 @@
         <v>13.72110753025661</v>
       </c>
       <c r="CP203" t="n">
-        <v>12.65777058962406</v>
+        <v>12.65695458962406</v>
       </c>
       <c r="CQ203" t="n">
         <v>9.987997258941411</v>
@@ -59978,7 +59978,7 @@
         <v>15.83067495190395</v>
       </c>
       <c r="CP204" t="n">
-        <v>8.679136716816178</v>
+        <v>8.678320716816177</v>
       </c>
       <c r="CQ204" t="n">
         <v>13.27911277768382</v>
@@ -60269,7 +60269,7 @@
         <v>14.59136005033485</v>
       </c>
       <c r="CP205" t="n">
-        <v>-5.234150382553143</v>
+        <v>-5.234966382553144</v>
       </c>
       <c r="CQ205" t="n">
         <v>11.96046395971465</v>
@@ -60560,7 +60560,7 @@
         <v>31.58645478694182</v>
       </c>
       <c r="CP206" t="n">
-        <v>14.68519367723979</v>
+        <v>14.68437767723979</v>
       </c>
       <c r="CQ206" t="n">
         <v>10.55792970680097</v>
@@ -60851,7 +60851,7 @@
         <v>10.37865383749045</v>
       </c>
       <c r="CP207" t="n">
-        <v>-5.49186757033482</v>
+        <v>-5.492683570334821</v>
       </c>
       <c r="CQ207" t="n">
         <v>13.07546376135915</v>
@@ -61142,7 +61142,7 @@
         <v>14.60826598591838</v>
       </c>
       <c r="CP208" t="n">
-        <v>12.69373862306411</v>
+        <v>12.69292262306411</v>
       </c>
       <c r="CQ208" t="n">
         <v>8.96691247626371</v>
@@ -61433,7 +61433,7 @@
         <v>13.87518418947919</v>
       </c>
       <c r="CP209" t="n">
-        <v>11.94149745695785</v>
+        <v>11.94068145695785</v>
       </c>
       <c r="CQ209" t="n">
         <v>9.93530756681055</v>
@@ -61724,7 +61724,7 @@
         <v>39.98836835342111</v>
       </c>
       <c r="CP210" t="n">
-        <v>11.01462997775118</v>
+        <v>11.01381397775118</v>
       </c>
       <c r="CQ210" t="n">
         <v>13.95370293840411</v>
@@ -62015,7 +62015,7 @@
         <v>19.95006257402531</v>
       </c>
       <c r="CP211" t="n">
-        <v>3.737026023984297</v>
+        <v>3.736210023984296</v>
       </c>
       <c r="CQ211" t="n">
         <v>10.56171366083252</v>
@@ -62306,7 +62306,7 @@
         <v>9.412308373363034</v>
       </c>
       <c r="CP212" t="n">
-        <v>13.12805814294775</v>
+        <v>13.12724214294775</v>
       </c>
       <c r="CQ212" t="n">
         <v>15.09683688541417</v>
@@ -62597,7 +62597,7 @@
         <v>13.93753671408548</v>
       </c>
       <c r="CP213" t="n">
-        <v>10.67441825253062</v>
+        <v>10.67360225253062</v>
       </c>
       <c r="CQ213" t="n">
         <v>11.13254430784615</v>
@@ -62888,7 +62888,7 @@
         <v>9.118928554571109</v>
       </c>
       <c r="CP214" t="n">
-        <v>14.78636066175928</v>
+        <v>14.78554466175928</v>
       </c>
       <c r="CQ214" t="n">
         <v>11.8666166193725</v>
@@ -63179,7 +63179,7 @@
         <v>12.6010453502041</v>
       </c>
       <c r="CP215" t="n">
-        <v>-5.512930903295605</v>
+        <v>-5.513746903295606</v>
       </c>
       <c r="CQ215" t="n">
         <v>9.707291037511585</v>
@@ -63470,7 +63470,7 @@
         <v>16.61957072632329</v>
       </c>
       <c r="CP216" t="n">
-        <v>7.624768465316564</v>
+        <v>7.623952465316564</v>
       </c>
       <c r="CQ216" t="n">
         <v>9.917844808650667</v>
@@ -63761,7 +63761,7 @@
         <v>15.94850967186459</v>
       </c>
       <c r="CP217" t="n">
-        <v>10.55753632452999</v>
+        <v>10.55672032452999</v>
       </c>
       <c r="CQ217" t="n">
         <v>11.0228142722327</v>
@@ -64052,7 +64052,7 @@
         <v>11.63652355024853</v>
       </c>
       <c r="CP218" t="n">
-        <v>12.49995246510948</v>
+        <v>21.95593646510948</v>
       </c>
       <c r="CQ218" t="n">
         <v>13.70656665032598</v>
@@ -64343,7 +64343,7 @@
         <v>12.66484789160534</v>
       </c>
       <c r="CP219" t="n">
-        <v>16.826120408112</v>
+        <v>16.825304408112</v>
       </c>
       <c r="CQ219" t="n">
         <v>10.19360834955061</v>
@@ -64634,7 +64634,7 @@
         <v>16.59570000753079</v>
       </c>
       <c r="CP220" t="n">
-        <v>7.399660975528144</v>
+        <v>7.398844975528144</v>
       </c>
       <c r="CQ220" t="n">
         <v>9.738820257758634</v>
@@ -64925,7 +64925,7 @@
         <v>16.58232910575169</v>
       </c>
       <c r="CP221" t="n">
-        <v>-7.077594964152532</v>
+        <v>-7.078410964152533</v>
       </c>
       <c r="CQ221" t="n">
         <v>12.33220810380494</v>
@@ -65216,7 +65216,7 @@
         <v>16.60166260710023</v>
       </c>
       <c r="CP222" t="n">
-        <v>7.497462130272039</v>
+        <v>7.496646130272039</v>
       </c>
       <c r="CQ222" t="n">
         <v>9.783131929639977</v>
@@ -65507,7 +65507,7 @@
         <v>16.60580851993685</v>
       </c>
       <c r="CP223" t="n">
-        <v>7.432325855536475</v>
+        <v>7.431509855536475</v>
       </c>
       <c r="CQ223" t="n">
         <v>9.814101269263803</v>
@@ -65798,7 +65798,7 @@
         <v>16.64910034294081</v>
       </c>
       <c r="CP224" t="n">
-        <v>8.52148333818938</v>
+        <v>8.52066733818938</v>
       </c>
       <c r="CQ224" t="n">
         <v>10.14543350399165</v>
@@ -66089,7 +66089,7 @@
         <v>16.59733531790025</v>
       </c>
       <c r="CP225" t="n">
-        <v>7.361996849620143</v>
+        <v>7.361180849620142</v>
       </c>
       <c r="CQ225" t="n">
         <v>9.750946557151352</v>
@@ -66380,7 +66380,7 @@
         <v>13.5161533459285</v>
       </c>
       <c r="CP226" t="n">
-        <v>-0.5649360575438225</v>
+        <v>8.891047942456183</v>
       </c>
       <c r="CQ226" t="n">
         <v>16.38580986458334</v>
@@ -66671,7 +66671,7 @@
         <v>11.06847301517518</v>
       </c>
       <c r="CP227" t="n">
-        <v>16.17062173172836</v>
+        <v>16.16980573172836</v>
       </c>
       <c r="CQ227" t="n">
         <v>10.49059686518084</v>
@@ -66962,7 +66962,7 @@
         <v>14.91559755676484</v>
       </c>
       <c r="CP228" t="n">
-        <v>-7.594052897432835</v>
+        <v>-7.594868897432836</v>
       </c>
       <c r="CQ228" t="n">
         <v>11.576092290965</v>
@@ -67253,7 +67253,7 @@
         <v>14.48454620736778</v>
       </c>
       <c r="CP229" t="n">
-        <v>9.780058118562511</v>
+        <v>9.779242118562511</v>
       </c>
       <c r="CQ229" t="n">
         <v>9.863261762207998</v>

</xml_diff>